<commit_message>
Fixed some issue and cleaned up the project.
Added chrome and gecko driver within the project folder.

Signed-off-by: Nashed <798014@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/java/co/ExcelDataPackage/SeleniumQBEValues.xlsx
+++ b/src/main/java/co/ExcelDataPackage/SeleniumQBEValues.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\798014\eclipse-workspace\GradAssignmentSelenium\src\main\java\co\ExcelDataPackage\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="6000"/>
   </bookViews>
   <sheets>
     <sheet name="DataValues" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -401,7 +397,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>